<commit_message>
new results and plots
</commit_message>
<xml_diff>
--- a/project/Res-Analysis/Result-Analysis.xlsx
+++ b/project/Res-Analysis/Result-Analysis.xlsx
@@ -4,14 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="2520" windowWidth="13980" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="0" windowWidth="27560" windowHeight="17540" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Precision-HighRisk-AllFeatures" sheetId="1" r:id="rId1"/>
-    <sheet name="Feature-Selection-AUROC" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature-Selection-AUROC-90" sheetId="2" r:id="rId2"/>
     <sheet name="Precision-LessRisk-AllFeat" sheetId="3" r:id="rId3"/>
     <sheet name="Recall-HighRisk-AllFeat" sheetId="4" r:id="rId4"/>
     <sheet name="Recall-LowRisk-AllFeat" sheetId="5" r:id="rId5"/>
+    <sheet name="Feature-Selection-50Percent" sheetId="6" r:id="rId6"/>
+    <sheet name="10-Cross-Validation" sheetId="7" r:id="rId7"/>
+    <sheet name="5-Cross-Validation" sheetId="8" r:id="rId8"/>
+    <sheet name="Cross-Fold-AUROC" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
   <si>
     <t>Training Size</t>
   </si>
@@ -51,15 +55,62 @@
   <si>
     <t xml:space="preserve">90% training set </t>
   </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>RandomFor</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Ten</t>
+  </si>
+  <si>
+    <t>AUROC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -82,13 +133,59 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="23">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -120,22 +217,20 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
               <a:t>Precision Score of Highly</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> Susceptible </a:t>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t> Risky Applications</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Android</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> Applications</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600"/>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -648,11 +743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2138485016"/>
-        <c:axId val="-2111211304"/>
+        <c:axId val="-2129754360"/>
+        <c:axId val="-2129747096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2138485016"/>
+        <c:axId val="-2129754360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -686,7 +781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111211304"/>
+        <c:crossAx val="-2129747096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -694,11 +789,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111211304"/>
+        <c:axId val="-2129747096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -726,10 +821,628 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2138485016"/>
+        <c:crossAx val="-2129754360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>Five-Fold</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t> Cross Validation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$B$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5-Cross-Validation'!$B$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct40">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$B$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5-Cross-Validation'!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2070965896"/>
+        <c:axId val="-2105852200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2070965896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Classifiers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2105852200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2105852200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:latin typeface="Times New Roman"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Recall</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t> Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Times New Roman"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2070965896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>Area</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t> Under ROC For Five and Ten Folded Validations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cross-Fold-AUROC'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Five</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Cross-Fold-AUROC'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cross-Fold-AUROC'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.633900928793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.497180451128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.529411764706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.606368863335</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.587295444494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Cross-Fold-AUROC'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct40">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Cross-Fold-AUROC'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Cross-Fold-AUROC'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.633900928793</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.497180451128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.529411764706</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.604489164087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.587295444494</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2113573640"/>
+        <c:axId val="-2068032264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2113573640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:latin typeface="Times New Roman"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Classifiers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2068032264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2068032264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>AUROC</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113573640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -790,7 +1503,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -804,7 +1516,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Feature-Selection-AUROC'!$B$1</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -814,7 +1526,173 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cmpd="sng">
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature-Selection-AUROC-90'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-AUROC-90'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-AUROC-90'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GNB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -825,11 +1703,12 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$A$2:$A$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -898,176 +1777,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$B$2:$B$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.49</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Feature-Selection-AUROC'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GNB</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="lgDashDotDot"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="plus"/>
-            <c:size val="5"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$C$2:$C$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$C$2:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1141,7 +1851,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Feature-Selection-AUROC'!$D$1</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1155,7 +1865,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$A$2:$A$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1224,7 +1934,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$D$2:$D$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1298,7 +2008,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Feature-Selection-AUROC'!$E$1</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1308,19 +2018,20 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cmpd="sng">
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
+              <a:prstDash val="sysDash"/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="x"/>
             <c:size val="5"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$A$2:$A$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1389,7 +2100,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$E$2:$E$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$E$2:$E$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1463,7 +2174,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Feature-Selection-AUROC'!$F$1</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1473,19 +2184,20 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cmpd="sng">
+            <a:ln w="12700" cmpd="sng">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
+              <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$A$2:$A$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1554,7 +2266,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Feature-Selection-AUROC'!$F$2:$F$21</c:f>
+              <c:f>'Feature-Selection-AUROC-90'!$F$2:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1633,11 +2345,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2123943528"/>
-        <c:axId val="2123843000"/>
+        <c:axId val="-2125911272"/>
+        <c:axId val="-2125905240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2123943528"/>
+        <c:axId val="-2125911272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,14 +2382,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123843000"/>
+        <c:crossAx val="-2125905240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1685,7 +2396,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123843000"/>
+        <c:axId val="-2125905240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,21 +2430,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123943528"/>
+        <c:crossAx val="-2125911272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1795,11 +2504,13 @@
             <a:r>
               <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
                 <a:effectLst/>
+                <a:latin typeface="Times New Roman"/>
               </a:rPr>
-              <a:t>Precision Score of Less Susceptible Android Applications</a:t>
+              <a:t>Precision Score of Less Risky Applications</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1600">
               <a:effectLst/>
+              <a:latin typeface="Times New Roman"/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
@@ -2313,11 +3024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2123903576"/>
-        <c:axId val="2128653880"/>
+        <c:axId val="-2129071384"/>
+        <c:axId val="-2129065512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2123903576"/>
+        <c:axId val="-2129071384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,7 +3062,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128653880"/>
+        <c:crossAx val="-2129065512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2359,7 +3070,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2128653880"/>
+        <c:axId val="-2129065512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2391,7 +3102,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123903576"/>
+        <c:crossAx val="-2129071384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -2459,18 +3170,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
                 <a:effectLst/>
+                <a:latin typeface="Times New Roman"/>
               </a:rPr>
-              <a:t>Recall Score of Highly Susceptible Android Applications</a:t>
+              <a:t>Recall Score of High Risky Applications</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1600">
               <a:effectLst/>
+              <a:latin typeface="Times New Roman"/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2979,11 +3691,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2107462888"/>
-        <c:axId val="-2107562472"/>
+        <c:axId val="-2129003320"/>
+        <c:axId val="-2128997448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2107462888"/>
+        <c:axId val="-2129003320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3010,14 +3722,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107562472"/>
+        <c:crossAx val="-2128997448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3025,7 +3736,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107562472"/>
+        <c:axId val="-2128997448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3055,14 +3766,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107462888"/>
+        <c:crossAx val="-2129003320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.1"/>
@@ -3070,7 +3780,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3130,18 +3839,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
                 <a:effectLst/>
+                <a:latin typeface="Times New Roman"/>
               </a:rPr>
-              <a:t>Recall Score of Less Susceptible Android Applications</a:t>
+              <a:t>Recall Score of Less Risky Applications</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
+            <a:endParaRPr lang="en-US" sz="1600">
               <a:effectLst/>
+              <a:latin typeface="Times New Roman"/>
             </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3650,11 +4360,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2108678664"/>
-        <c:axId val="-2111660504"/>
+        <c:axId val="-2128940072"/>
+        <c:axId val="-2128934200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2108678664"/>
+        <c:axId val="-2128940072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,14 +4391,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111660504"/>
+        <c:crossAx val="-2128934200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3696,7 +4405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111660504"/>
+        <c:axId val="-2128934200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3726,6 +4435,651 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2128940072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>Count</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t> of Features Might Not Effect Classifier Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-50Percent'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KNN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-50Percent'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5676</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5676</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56583</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5621</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-50Percent'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GNB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-50Percent'!$C$2:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.496</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4533</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.352</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.325</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.50133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4994</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5255</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5311</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.533</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.54424</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.54424</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.54424</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-50Percent'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-50Percent'!$D$2:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.571428</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-50Percent'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RandomForest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="lgDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-50Percent'!$E$2:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.772</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7049</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70122</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.706823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71055</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.71428</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.706823</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.70309</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7086</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.71055</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.71242</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.64099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.70495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature-Selection-50Percent'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cmpd="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature-Selection-50Percent'!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.772654584222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.691897654584</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6922</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.702158</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.701226012793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.689</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.684</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68346</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.689385</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68985</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.695628997868</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.706823027719</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.710554371002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.710554371002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.706823027719</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.70868869936</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70868869936</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.704957356077</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.703091684435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2128878712"/>
+        <c:axId val="-2128872776"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2128878712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Count</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Features</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2128872776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2128872776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Area</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Under the Curve</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -3733,10 +5087,941 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108678664"/>
+        <c:crossAx val="-2128878712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>10</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>-Fold Cross Validation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10-Cross-Validation'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct40">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10-Cross-Validation'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2130042488"/>
+        <c:axId val="-2130038664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2130042488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Classifiers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2130038664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2130038664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Precision</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t> Scores</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Times New Roman"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2130042488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>10-Fold</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t> Cross Validation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$B$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10-Cross-Validation'!$B$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct40">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10-Cross-Validation'!$B$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10-Cross-Validation'!$B$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2071395320"/>
+        <c:axId val="-2071472056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2071395320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Classifiers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2071472056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2071472056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:latin typeface="Times New Roman"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Recall</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t> Score</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Times New Roman"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2071395320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman"/>
+              </a:rPr>
+              <a:t>Five-Fold Cross Validation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct90">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5-Cross-Validation'!$B$2:$F$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="pct40">
+              <a:fgClr>
+                <a:prstClr val="black"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:prstClr val="white"/>
+              </a:bgClr>
+            </a:pattFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'5-Cross-Validation'!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>CART</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GNB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>RandomFor</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'5-Cross-Validation'!$B$3:$F$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2070995384"/>
+        <c:axId val="-2071113160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2070995384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Classifiers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2071113160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2071113160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t>Precision</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:latin typeface="Times New Roman"/>
+                  </a:rPr>
+                  <a:t> Scores</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:latin typeface="Times New Roman"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2070995384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -3760,16 +6045,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3801,8 +6086,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
@@ -3831,15 +6116,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3905,15 +6190,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3921,6 +6206,210 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4261,8 +6750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4483,7 +6972,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4918,6 +7407,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4932,7 +7422,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5153,7 +7643,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5374,7 +7864,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5577,6 +8067,818 @@
       </c>
       <c r="F10">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E2">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="F2">
+        <v>0.77265458422199995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.498</v>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E3">
+        <v>0.70489999999999997</v>
+      </c>
+      <c r="F3">
+        <v>0.69189765458399999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.56759999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E4">
+        <v>0.70121999999999995</v>
+      </c>
+      <c r="F4">
+        <v>0.69220000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.56759999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E5">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F5">
+        <v>0.70215799999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.56583000000000006</v>
+      </c>
+      <c r="C6">
+        <v>0.496</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E6">
+        <v>0.70682299999999998</v>
+      </c>
+      <c r="F6">
+        <v>0.70122601279300001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.56583000000000006</v>
+      </c>
+      <c r="C7">
+        <v>0.496</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E7">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F7">
+        <v>0.68899999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.56583000000000006</v>
+      </c>
+      <c r="C8">
+        <v>0.45329999999999998</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E8">
+        <v>0.71055000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C9">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E9">
+        <v>0.71428000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.68345999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C10">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E10">
+        <v>0.70682299999999998</v>
+      </c>
+      <c r="F10">
+        <v>0.68938500000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C11">
+        <v>0.41249999999999998</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E11">
+        <v>0.70308999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C12">
+        <v>0.50133000000000005</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E12">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F12">
+        <v>0.68984999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C13">
+        <v>0.499</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E13">
+        <v>0.70860000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.69562899786800003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C14">
+        <v>0.49940000000000001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E14">
+        <v>0.71055000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.70682302771899996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C15">
+        <v>0.52549999999999997</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F15">
+        <v>0.71055437100200003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C16">
+        <v>0.53110000000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F16">
+        <v>0.71055437100200003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C17">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F17">
+        <v>0.70682302771899996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C18">
+        <v>0.54423999999999995</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F18">
+        <v>0.70868869936000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C19">
+        <v>0.54423999999999995</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.71242000000000005</v>
+      </c>
+      <c r="F19">
+        <v>0.70868869936000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C20">
+        <v>0.54423999999999995</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.64098999999999995</v>
+      </c>
+      <c r="F20">
+        <v>0.70495735607700005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.56210000000000004</v>
+      </c>
+      <c r="C21">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.57142800000000005</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.70494999999999997</v>
+      </c>
+      <c r="F21">
+        <v>0.70309168443500003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.98</v>
+      </c>
+      <c r="C2">
+        <v>0.97</v>
+      </c>
+      <c r="D2">
+        <v>0.97</v>
+      </c>
+      <c r="E2">
+        <v>0.98</v>
+      </c>
+      <c r="F2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.35</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.22</v>
+      </c>
+      <c r="F3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0.98</v>
+      </c>
+      <c r="C2">
+        <v>0.97</v>
+      </c>
+      <c r="D2">
+        <v>0.97</v>
+      </c>
+      <c r="E2">
+        <v>0.98</v>
+      </c>
+      <c r="F2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.26</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.25</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.99</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>0.63390092879299997</v>
+      </c>
+      <c r="C2">
+        <v>0.49718045112800002</v>
+      </c>
+      <c r="D2">
+        <v>0.52941176470600004</v>
+      </c>
+      <c r="E2">
+        <v>0.60636886333499995</v>
+      </c>
+      <c r="F2">
+        <v>0.58729544449399995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>0.63390092879299997</v>
+      </c>
+      <c r="C3">
+        <v>0.49718045112800002</v>
+      </c>
+      <c r="D3">
+        <v>0.52941176470600004</v>
+      </c>
+      <c r="E3">
+        <v>0.60448916408700004</v>
+      </c>
+      <c r="F3">
+        <v>0.58729544449399995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>